<commit_message>
Added result percenteges in text file
</commit_message>
<xml_diff>
--- a/global results/globalSupersenseUniquesLemmasPercentages.xlsx
+++ b/global results/globalSupersenseUniquesLemmasPercentages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dizertatie-bookNLP\global results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78E7A62-D950-4E1F-B6DB-9D5DD2005331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90FE215-BB16-48FE-8BB2-BF4773534B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>noun.act</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>gibson</t>
+  </si>
+  <si>
+    <t>supersense_category</t>
   </si>
 </sst>
 </file>
@@ -477,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -487,6 +490,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
       <c r="B1" t="s">
         <v>42</v>
       </c>

</xml_diff>